<commit_message>
MB and PS in 3rd and 4th periods interchanged; 10C ROT SS given taken from RK and given to PS in 4th period
</commit_message>
<xml_diff>
--- a/Timetable.xlsx
+++ b/Timetable.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CLASSWISE" sheetId="1" state="visible" r:id="rId3"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="562">
   <si>
     <t xml:space="preserve">Period\
 Class</t>
@@ -147,13 +147,13 @@
   </si>
   <si>
     <t xml:space="preserve">CS (1-2) JK
-SS (3) MB
+ENG (3) PS
 PBI (4-6) GK</t>
   </si>
   <si>
     <t xml:space="preserve">HI (1, 3) MA
 CS (2) JK
-ENG (4) PS
+SS (4) MB
 SCI (5) RI
 PBI (6) GK</t>
   </si>
@@ -566,7 +566,7 @@
   </si>
   <si>
     <t xml:space="preserve">ROT NSQF-CG-YNV (2) RK
-ROT SS (4) RK
+ROT SS (4) PS
 MATH (1, 3, 5-6) SH</t>
   </si>
   <si>
@@ -800,7 +800,7 @@
 CS (6) JK</t>
   </si>
   <si>
-    <t xml:space="preserve">Last updated on Fri Oct  3 14:04:00 2025</t>
+    <t xml:space="preserve">Last updated on Wed Oct  8 14:41:25 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Name</t>
@@ -844,9 +844,6 @@
   <si>
     <t xml:space="preserve">11A (2) ENG
 12A (5-6) ENG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1: 3, 2: 4, 3: 4, 4: 4, 5: 7, 6: 7</t>
   </si>
   <si>
     <t xml:space="preserve">Moti Ram, MR</t>
@@ -884,9 +881,6 @@
   <si>
     <t xml:space="preserve">11A (1, 6) POL
 11B (3-5) POL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1: 7, 2: 6, 3: 5, 4: 5, 5: 6, 6: 6</t>
   </si>
   <si>
     <t xml:space="preserve">Sunil Kumar, SK</t>
@@ -929,9 +923,6 @@
 11B (3-5) MATH</t>
   </si>
   <si>
-    <t xml:space="preserve">1: 5, 2: 5, 3: 4, 4: 4, 5: 4, 6: 5</t>
-  </si>
-  <si>
     <t xml:space="preserve">Angrej Singh, AS</t>
   </si>
   <si>
@@ -968,9 +959,6 @@
 12B (5) HIS</t>
   </si>
   <si>
-    <t xml:space="preserve">1: 5, 2: 4, 3: 6, 4: 5, 5: 7, 6: 7</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mukesh Rajoria, MU</t>
   </si>
   <si>
@@ -1005,9 +993,6 @@
 12B (1-4) PE</t>
   </si>
   <si>
-    <t xml:space="preserve">1: 7, 2: 5, 3: 6, 4: 6, 5: 5, 6: 3</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mohit Kumar, MK</t>
   </si>
   <si>
@@ -1041,9 +1026,6 @@
     <t xml:space="preserve">10A (2) MATH</t>
   </si>
   <si>
-    <t xml:space="preserve">1: 4, 2: 5, 3: 5, 4: 5, 5: 2, 6: 5</t>
-  </si>
-  <si>
     <t xml:space="preserve">Shunty Kumar, SH</t>
   </si>
   <si>
@@ -1074,9 +1056,6 @@
 11A (5) HIS</t>
   </si>
   <si>
-    <t xml:space="preserve">1: 4, 2: 4, 3: 4, 4: 5, 5: 5, 6: 4</t>
-  </si>
-  <si>
     <t xml:space="preserve">Rajiv Narang, RN</t>
   </si>
   <si>
@@ -1112,9 +1091,6 @@
     <t xml:space="preserve">8B (2) MATH
 9A (3) MATH
 7A (4) MATH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1: 5, 2: 5, 3: 4, 4: 4, 5: 5, 6: 4</t>
   </si>
   <si>
     <t xml:space="preserve">Raman Sama, RS</t>
@@ -1150,9 +1126,6 @@
 9C (6) MATH</t>
   </si>
   <si>
-    <t xml:space="preserve">1: 6, 2: 5, 3: 4, 4: 3, 5: 4, 6: 5</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gurwinder Kaur, GK</t>
   </si>
   <si>
@@ -1189,9 +1162,6 @@
 9C (6) PBI</t>
   </si>
   <si>
-    <t xml:space="preserve">1: 5, 2: 6, 3: 7, 4: 6, 5: 6, 6: 6</t>
-  </si>
-  <si>
     <t xml:space="preserve">Anju Bala, AB</t>
   </si>
   <si>
@@ -1229,9 +1199,6 @@
 9A (5-6) PBI</t>
   </si>
   <si>
-    <t xml:space="preserve">1: 6, 2: 6, 3: 6, 4: 7, 5: 6, 6: 5</t>
-  </si>
-  <si>
     <t xml:space="preserve">Vijay Singh, VS</t>
   </si>
   <si>
@@ -1264,9 +1231,6 @@
     <t xml:space="preserve">8A (3) SCI
 6A (5) SCI
 10C (6) SCI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1: 2, 2: 6, 3: 6, 4: 5, 5: 5, 6: 4</t>
   </si>
   <si>
     <t xml:space="preserve">Sunita Devi, SU</t>
@@ -1306,9 +1270,6 @@
 9A (4) SCI</t>
   </si>
   <si>
-    <t xml:space="preserve">1: 4, 2: 6, 3: 6, 4: 5, 5: 4, 6: 4</t>
-  </si>
-  <si>
     <t xml:space="preserve">Reetika, RI</t>
   </si>
   <si>
@@ -1348,9 +1309,6 @@
 7A (5-6) SCI</t>
   </si>
   <si>
-    <t xml:space="preserve">1: 4, 2: 6, 3: 4, 4: 7, 5: 4, 6: 5</t>
-  </si>
-  <si>
     <t xml:space="preserve">Meenu Bala, MB</t>
   </si>
   <si>
@@ -1362,11 +1320,11 @@
   </si>
   <si>
     <t xml:space="preserve">6A (2) SS
-7A (3) SS
 10C (6) ENG</t>
   </si>
   <si>
-    <t xml:space="preserve">10A (2) ROT NSQF-CG-YNV</t>
+    <t xml:space="preserve">10A (2) ROT NSQF-CG-YNV
+7A (4) SS</t>
   </si>
   <si>
     <t xml:space="preserve">7A (1-2, 6) SS</t>
@@ -1382,9 +1340,6 @@
   <si>
     <t xml:space="preserve">7A (1-2) SS
 6B (3-6) SS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1: 5, 2: 7, 3: 5, 4: 4, 5: 4, 6: 7</t>
   </si>
   <si>
     <t xml:space="preserve">Sanjay Solanki, SN</t>
@@ -1422,9 +1377,6 @@
     <t xml:space="preserve">8B (3, 5-6) ENG</t>
   </si>
   <si>
-    <t xml:space="preserve">1: 5, 2: 2, 3: 5, 4: 5, 5: 5, 6: 7</t>
-  </si>
-  <si>
     <t xml:space="preserve">Parmila, PR</t>
   </si>
   <si>
@@ -1464,9 +1416,6 @@
 10A (5) SS</t>
   </si>
   <si>
-    <t xml:space="preserve">1: 6, 2: 4, 3: 6, 4: 6, 5: 6, 6: 4</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pratibha Setia, PS</t>
   </si>
   <si>
@@ -1477,8 +1426,11 @@
 7A (5-6) ENG</t>
   </si>
   <si>
+    <t xml:space="preserve">7A (3) ENG</t>
+  </si>
+  <si>
     <t xml:space="preserve">8A (3) SS
-7A (4) ENG
+10C (4) ROT SS
 9B (5) SS
 9B (6) ROT SS</t>
   </si>
@@ -1496,9 +1448,6 @@
   <si>
     <t xml:space="preserve">9B (1, 5-6) SS
 10C (2-4) SS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1: 5, 2: 4, 3: 5, 4: 5, 5: 6, 6: 5</t>
   </si>
   <si>
     <t xml:space="preserve">Priyanka, PY</t>
@@ -1539,9 +1488,6 @@
 10B (5-6) SS</t>
   </si>
   <si>
-    <t xml:space="preserve">1: 6, 2: 4, 3: 6, 4: 5, 5: 6, 6: 5</t>
-  </si>
-  <si>
     <t xml:space="preserve">Maya, MA</t>
   </si>
   <si>
@@ -1576,9 +1522,6 @@
 7B (6) HI</t>
   </si>
   <si>
-    <t xml:space="preserve">1: 5, 2: 5, 3: 5, 4: 5, 5: 4, 6: 4</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ratan Lal, RL</t>
   </si>
   <si>
@@ -1613,9 +1556,6 @@
 6A (6) HI</t>
   </si>
   <si>
-    <t xml:space="preserve">1: 7, 2: 4, 3: 3, 4: 4, 5: 5, 6: 4</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ravi Kumar, RK</t>
   </si>
   <si>
@@ -1625,8 +1565,7 @@
   <si>
     <t xml:space="preserve">8B (1) AG
 10C (2) ROT NSQF-CG-YNV
-10A (4) ROT SS
-10C (4) ROT SS</t>
+10A (4) ROT SS</t>
   </si>
   <si>
     <t xml:space="preserve">10A (1-6) PE
@@ -1640,9 +1579,6 @@
   </si>
   <si>
     <t xml:space="preserve">11B (5) HIS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1: 4, 2: 4, 3: 2, 4: 4, 5: 3, 6: 3</t>
   </si>
   <si>
     <t xml:space="preserve">Daulat Ram, DR</t>
@@ -1681,9 +1617,6 @@
 8A (5) PE</t>
   </si>
   <si>
-    <t xml:space="preserve">1: 2, 2: 4, 3: 4, 4: 3, 5: 5, 6: 4</t>
-  </si>
-  <si>
     <t xml:space="preserve">Jaspreet Kaur, JK</t>
   </si>
   <si>
@@ -1727,9 +1660,6 @@
 12B (6) CS</t>
   </si>
   <si>
-    <t xml:space="preserve">1: 4, 2: 6, 3: 5, 4: 5, 5: 7, 6: 5</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sachin Kumar, SJ</t>
   </si>
   <si>
@@ -1765,9 +1695,6 @@
 7B (4-5) CS</t>
   </si>
   <si>
-    <t xml:space="preserve">1: 5, 2: 6, 3: 5, 4: 6, 5: 4, 6: 6</t>
-  </si>
-  <si>
     <t xml:space="preserve">Anchal Rani, AR</t>
   </si>
   <si>
@@ -1800,9 +1727,6 @@
 12B (1-4) IT</t>
   </si>
   <si>
-    <t xml:space="preserve">1: 7, 2: 5, 3: 6, 4: 6, 5: 4, 6: 3</t>
-  </si>
-  <si>
     <t xml:space="preserve">Joginderpal, JP</t>
   </si>
   <si>
@@ -1832,9 +1756,6 @@
 12B (1-4) PLB</t>
   </si>
   <si>
-    <t xml:space="preserve">1: 6, 2: 5, 3: 6, 4: 6, 5: 4, 6: 3</t>
-  </si>
-  <si>
     <t xml:space="preserve">Free Teachers Sheet</t>
   </si>
   <si>
@@ -1925,22 +1846,22 @@
     <t xml:space="preserve">RK:6, RL:5, DR:4, SJ:3, JK:3, MA:3, SN:3, PY:2, AR:2, JP:2</t>
   </si>
   <si>
-    <t xml:space="preserve">RK:6, RL:5, SH:4, RN:4, SK:4, MB:3, PS:3, MR:3, PR:2, VS:2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RK:6, RS:4, AA:4, SJ:3, JK:3, MK:3, PS:3, MA:3, SN:3, AS:2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RK:6, RL:5, RI:4, SK:4, AA:4, MB:3, JK:3, MK:3, AB:2, AR:2, JP:2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RS:4, SH:4, RN:4, SK:4, MB:3, MA:3, MR:3, VS:2, SU:2, MU:2, AS:2</t>
+    <t xml:space="preserve">RK:6, RL:5, MB:4, SH:4, RN:4, SK:4, MR:3, PR:2, VS:2, PS:2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RK:6, RS:4, MB:4, AA:4, SJ:3, JK:3, MK:3, MA:3, SN:3, AS:2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RK:6, RL:5, MB:4, RI:4, SK:4, AA:4, JK:3, MK:3, AB:2, AR:2, JP:2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS:4, MB:4, SH:4, RN:4, SK:4, MA:3, MR:3, VS:2, SU:2, MU:2, AS:2</t>
   </si>
   <si>
     <t xml:space="preserve">RL:5, RS:4, DR:4, RN:4, RI:4, AA:4, AB:2, PR:2, SU:2, PY:2, MU:2</t>
   </si>
   <si>
-    <t xml:space="preserve">RK:6, DR:4, SH:4, RN:4, RI:4, SK:4, SJ:3, PS:3, SN:3, MR:3</t>
+    <t xml:space="preserve">RK:6, DR:4, SH:4, RN:4, RI:4, SK:4, SJ:3, SN:3, MR:3, PS:2</t>
   </si>
   <si>
     <t xml:space="preserve">RK:6, RL:5, RS:4, DR:4, SH:4, RI:4, AA:4, MK:3, GK:1</t>
@@ -1952,16 +1873,16 @@
     <t xml:space="preserve">DR:5, RK:5, RL:3, JK:3, MA:3, SN:3, PY:3, SJ:2, AR:2, JP:2</t>
   </si>
   <si>
-    <t xml:space="preserve">DR:5, RK:5, MB:4, RN:4, SK:4, AA:4, VS:3, SH:3, PS:3, MR:3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RS:6, RK:5, MB:4, RN:4, SK:4, MK:3, PS:3, MA:3, MR:3, AS:3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RS:6, DR:5, MB:4, RN:4, SK:4, AA:4, MA:3, PR:2, GK:2, SU:2, AR:2, JP:2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RS:6, MB:4, VS:3, MR:3, AS:3, SJ:2, GK:2, SU:2, MU:2, RI:1</t>
+    <t xml:space="preserve">DR:5, RK:5, RN:4, SK:4, AA:4, VS:3, MB:3, SH:3, PS:3, MR:3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS:6, RK:5, RN:4, SK:4, MB:3, MK:3, PS:3, MA:3, MR:3, AS:3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS:6, DR:5, RN:4, SK:4, AA:4, MA:3, PR:2, GK:2, SU:2, AR:2, JP:2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS:6, VS:3, MB:3, MR:3, AS:3, SJ:2, GK:2, SU:2, MU:2, RI:1</t>
   </si>
   <si>
     <t xml:space="preserve">RS:6, DR:5, RL:3, JK:3, MK:3, SN:3, PY:3, AS:3, PR:2, MU:2</t>
@@ -2025,9 +1946,6 @@
   </si>
   <si>
     <t xml:space="preserve">RK:5, AR:5, JP:5, MU:5, DR:4, PR:4, SU:4, RN:4, MK:3, RS:2, AS:1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last updated on Fri Oct  3 14:04:01 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Teacher</t>
@@ -3040,10 +2958,10 @@
   </sheetPr>
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.64453125" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3062,7 +2980,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1023" style="1" width="8.64"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="30.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="5" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3169,7 +3087,7 @@
       </c>
       <c r="L3" s="8"/>
     </row>
-    <row r="4" customFormat="false" ht="76.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="77.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
         <v>21</v>
       </c>
@@ -3701,10 +3619,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.1328125" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4801,693 +4719,653 @@
       <c r="J2" s="15" t="n">
         <v>29</v>
       </c>
-      <c r="K2" s="17" t="s">
-        <v>160</v>
-      </c>
+      <c r="K2" s="17"/>
     </row>
     <row r="3" customFormat="false" ht="62.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="I3" s="7" t="s">
         <v>168</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>169</v>
       </c>
       <c r="J3" s="15" t="n">
         <v>35</v>
       </c>
-      <c r="K3" s="17" t="s">
-        <v>170</v>
-      </c>
+      <c r="K3" s="17"/>
     </row>
     <row r="4" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>172</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>174</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="I4" s="7" t="s">
         <v>176</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>178</v>
       </c>
       <c r="J4" s="15" t="n">
         <v>27</v>
       </c>
-      <c r="K4" s="17" t="s">
-        <v>179</v>
-      </c>
+      <c r="K4" s="17"/>
     </row>
     <row r="5" customFormat="false" ht="44.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="E5" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="F5" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="G5" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="H5" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="I5" s="7" t="s">
         <v>185</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>188</v>
       </c>
       <c r="J5" s="15" t="n">
         <v>34</v>
       </c>
-      <c r="K5" s="17" t="s">
-        <v>189</v>
-      </c>
+      <c r="K5" s="17"/>
     </row>
     <row r="6" customFormat="false" ht="44.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="F6" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="G6" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="H6" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="I6" s="7" t="s">
         <v>194</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>198</v>
       </c>
       <c r="J6" s="15" t="n">
         <v>32</v>
       </c>
-      <c r="K6" s="17" t="s">
-        <v>199</v>
-      </c>
+      <c r="K6" s="17"/>
     </row>
     <row r="7" customFormat="false" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="G7" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="H7" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="I7" s="7" t="s">
         <v>203</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>208</v>
       </c>
       <c r="J7" s="15" t="n">
         <v>27</v>
       </c>
-      <c r="K7" s="17" t="s">
-        <v>209</v>
-      </c>
+      <c r="K7" s="17"/>
     </row>
     <row r="8" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>210</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>216</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="J8" s="15" t="n">
         <v>26</v>
       </c>
-      <c r="K8" s="17" t="s">
-        <v>218</v>
-      </c>
+      <c r="K8" s="17"/>
     </row>
     <row r="9" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="I9" s="7" t="s">
         <v>220</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>227</v>
       </c>
       <c r="J9" s="15" t="n">
         <v>27</v>
       </c>
-      <c r="K9" s="17" t="s">
-        <v>228</v>
-      </c>
+      <c r="K9" s="17"/>
     </row>
     <row r="10" customFormat="false" ht="57.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="15" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="I10" s="17"/>
       <c r="J10" s="15" t="n">
         <v>27</v>
       </c>
-      <c r="K10" s="17" t="s">
-        <v>237</v>
-      </c>
+      <c r="K10" s="17"/>
     </row>
     <row r="11" customFormat="false" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="18" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="J11" s="15" t="n">
         <v>36</v>
       </c>
-      <c r="K11" s="17" t="s">
-        <v>247</v>
-      </c>
+      <c r="K11" s="17"/>
     </row>
     <row r="12" customFormat="false" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="15" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="J12" s="15" t="n">
         <v>36</v>
       </c>
-      <c r="K12" s="17" t="s">
-        <v>257</v>
-      </c>
+      <c r="K12" s="17"/>
     </row>
     <row r="13" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="15" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="J13" s="15" t="n">
         <v>28</v>
       </c>
-      <c r="K13" s="17" t="s">
-        <v>267</v>
-      </c>
+      <c r="K13" s="17"/>
     </row>
     <row r="14" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="15" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="J14" s="15" t="n">
         <v>29</v>
       </c>
-      <c r="K14" s="17" t="s">
-        <v>277</v>
-      </c>
+      <c r="K14" s="17"/>
     </row>
     <row r="15" customFormat="false" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="15" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="J15" s="15" t="n">
         <v>30</v>
       </c>
-      <c r="K15" s="17" t="s">
-        <v>287</v>
-      </c>
+      <c r="K15" s="17"/>
     </row>
     <row r="16" customFormat="false" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="15" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="J16" s="15" t="n">
         <v>32</v>
       </c>
-      <c r="K16" s="17" t="s">
-        <v>297</v>
-      </c>
+      <c r="K16" s="17"/>
     </row>
     <row r="17" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="15" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="J17" s="15" t="n">
         <v>29</v>
       </c>
-      <c r="K17" s="17" t="s">
-        <v>306</v>
-      </c>
+      <c r="K17" s="17"/>
     </row>
     <row r="18" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="15" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="J18" s="15" t="n">
         <v>32</v>
       </c>
-      <c r="K18" s="17" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="56.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K18" s="17"/>
+    </row>
+    <row r="19" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="15" t="s">
-        <v>317</v>
+        <v>300</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>318</v>
+        <v>301</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="D19" s="7"/>
+        <v>302</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>303</v>
+      </c>
       <c r="E19" s="7" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>324</v>
+        <v>308</v>
       </c>
       <c r="J19" s="15" t="n">
-        <v>30</v>
-      </c>
-      <c r="K19" s="17" t="s">
-        <v>325</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="K19" s="17"/>
     </row>
     <row r="20" customFormat="false" ht="81.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="15" t="s">
-        <v>326</v>
+        <v>309</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7" t="s">
-        <v>327</v>
+        <v>310</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>328</v>
+        <v>311</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>329</v>
+        <v>312</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>330</v>
+        <v>313</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>331</v>
+        <v>314</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>332</v>
+        <v>315</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>333</v>
+        <v>316</v>
       </c>
       <c r="J20" s="15" t="n">
         <v>32</v>
       </c>
-      <c r="K20" s="17" t="s">
-        <v>334</v>
-      </c>
+      <c r="K20" s="17"/>
     </row>
     <row r="21" customFormat="false" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="15" t="s">
-        <v>335</v>
+        <v>317</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="7" t="s">
-        <v>336</v>
+        <v>318</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>337</v>
+        <v>319</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>338</v>
+        <v>320</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>339</v>
+        <v>321</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>340</v>
+        <v>322</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>341</v>
+        <v>323</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>342</v>
+        <v>324</v>
       </c>
       <c r="J21" s="15" t="n">
         <v>28</v>
       </c>
-      <c r="K21" s="17" t="s">
-        <v>343</v>
-      </c>
+      <c r="K21" s="17"/>
     </row>
     <row r="22" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="15" t="s">
-        <v>344</v>
+        <v>325</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7" t="s">
-        <v>345</v>
+        <v>326</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>346</v>
+        <v>327</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>347</v>
+        <v>328</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>348</v>
+        <v>329</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>349</v>
+        <v>330</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>350</v>
+        <v>331</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>351</v>
+        <v>332</v>
       </c>
       <c r="J22" s="15" t="n">
         <v>27</v>
       </c>
-      <c r="K22" s="17" t="s">
-        <v>352</v>
-      </c>
+      <c r="K22" s="17"/>
       <c r="L22" s="19"/>
       <c r="M22" s="19"/>
       <c r="N22" s="19"/>
@@ -5502,199 +5380,187 @@
     </row>
     <row r="23" customFormat="false" ht="66" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="15" t="s">
-        <v>353</v>
+        <v>333</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
-        <v>354</v>
+        <v>334</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="7" t="s">
-        <v>355</v>
+        <v>335</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>356</v>
+        <v>336</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>357</v>
+        <v>337</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>358</v>
+        <v>338</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="15" t="n">
         <v>19</v>
       </c>
-      <c r="K23" s="17" t="s">
-        <v>359</v>
-      </c>
+      <c r="K23" s="17"/>
     </row>
     <row r="24" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="15" t="s">
-        <v>360</v>
+        <v>339</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="s">
-        <v>361</v>
+        <v>340</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>362</v>
+        <v>341</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>363</v>
+        <v>342</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>364</v>
+        <v>343</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>365</v>
+        <v>344</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>366</v>
+        <v>345</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>367</v>
+        <v>346</v>
       </c>
       <c r="J24" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="K24" s="17" t="s">
-        <v>368</v>
-      </c>
+      <c r="K24" s="17"/>
     </row>
     <row r="25" customFormat="false" ht="56.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="15" t="s">
-        <v>369</v>
+        <v>347</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>370</v>
+        <v>348</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>371</v>
+        <v>349</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>372</v>
+        <v>350</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>373</v>
+        <v>351</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>374</v>
+        <v>352</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>375</v>
+        <v>353</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>376</v>
+        <v>354</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>377</v>
+        <v>355</v>
       </c>
       <c r="J25" s="15" t="n">
         <v>32</v>
       </c>
-      <c r="K25" s="17" t="s">
-        <v>378</v>
-      </c>
+      <c r="K25" s="17"/>
     </row>
     <row r="26" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="20" t="s">
-        <v>379</v>
+        <v>356</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>380</v>
+        <v>357</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>381</v>
+        <v>358</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>382</v>
+        <v>359</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>383</v>
+        <v>360</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>384</v>
+        <v>361</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>385</v>
+        <v>362</v>
       </c>
       <c r="H26" s="21" t="s">
-        <v>386</v>
+        <v>363</v>
       </c>
       <c r="I26" s="21" t="s">
-        <v>387</v>
+        <v>364</v>
       </c>
       <c r="J26" s="20" t="n">
         <v>32</v>
       </c>
-      <c r="K26" s="17" t="s">
-        <v>388</v>
-      </c>
+      <c r="K26" s="17"/>
     </row>
     <row r="27" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="15" t="s">
-        <v>389</v>
+        <v>365</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
-        <v>390</v>
+        <v>366</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>391</v>
+        <v>367</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>392</v>
+        <v>368</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>393</v>
+        <v>369</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>394</v>
+        <v>370</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>395</v>
+        <v>371</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>396</v>
+        <v>372</v>
       </c>
       <c r="J27" s="20" t="n">
         <v>31</v>
       </c>
-      <c r="K27" s="7" t="s">
-        <v>397</v>
-      </c>
+      <c r="K27" s="7"/>
     </row>
     <row r="28" customFormat="false" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="15" t="s">
-        <v>398</v>
+        <v>373</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
-        <v>399</v>
+        <v>374</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>400</v>
+        <v>375</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7" t="s">
-        <v>401</v>
+        <v>376</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>402</v>
+        <v>377</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>403</v>
+        <v>378</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>404</v>
+        <v>379</v>
       </c>
       <c r="J28" s="15" t="n">
         <v>30</v>
       </c>
-      <c r="K28" s="7" t="s">
-        <v>405</v>
-      </c>
+      <c r="K28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="22"/>
@@ -7086,7 +6952,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75390625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7098,7 +6964,7 @@
     <row r="1" s="5" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="25"/>
       <c r="B1" s="26" t="s">
-        <v>406</v>
+        <v>380</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
@@ -7112,211 +6978,211 @@
     </row>
     <row r="2" customFormat="false" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="28" t="s">
-        <v>407</v>
+        <v>381</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>408</v>
+        <v>382</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>409</v>
+        <v>383</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>410</v>
+        <v>384</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>411</v>
+        <v>385</v>
       </c>
       <c r="F2" s="29" t="s">
-        <v>412</v>
+        <v>386</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>413</v>
+        <v>387</v>
       </c>
       <c r="H2" s="29" t="s">
-        <v>414</v>
+        <v>388</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>415</v>
+        <v>389</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="57.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="s">
-        <v>416</v>
+        <v>390</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>417</v>
+        <v>391</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>418</v>
+        <v>392</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>419</v>
+        <v>393</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>420</v>
+        <v>394</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>421</v>
+        <v>395</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>422</v>
+        <v>396</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>423</v>
+        <v>397</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>424</v>
+        <v>398</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="57.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="28" t="s">
-        <v>425</v>
+        <v>399</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>426</v>
+        <v>400</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>427</v>
+        <v>401</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>428</v>
+        <v>402</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>429</v>
+        <v>403</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>430</v>
+        <v>404</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>431</v>
+        <v>405</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>432</v>
+        <v>406</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>433</v>
+        <v>407</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="57.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="28" t="s">
-        <v>434</v>
+        <v>408</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>435</v>
+        <v>409</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>436</v>
+        <v>410</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>437</v>
+        <v>411</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>438</v>
+        <v>412</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>439</v>
+        <v>413</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>440</v>
+        <v>414</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>441</v>
+        <v>415</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>442</v>
+        <v>416</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="57.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="28" t="s">
-        <v>443</v>
+        <v>417</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>444</v>
+        <v>418</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>445</v>
+        <v>419</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>446</v>
+        <v>420</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>447</v>
+        <v>421</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>448</v>
+        <v>422</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>449</v>
+        <v>423</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>450</v>
+        <v>424</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>451</v>
+        <v>425</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="57.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="28" t="s">
-        <v>452</v>
+        <v>426</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>453</v>
+        <v>427</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>454</v>
+        <v>428</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>455</v>
+        <v>429</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>456</v>
+        <v>430</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>457</v>
+        <v>431</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>458</v>
+        <v>432</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>459</v>
+        <v>433</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>460</v>
+        <v>434</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="28" t="s">
-        <v>461</v>
+        <v>435</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>462</v>
+        <v>436</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>463</v>
+        <v>437</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>464</v>
+        <v>438</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>465</v>
+        <v>439</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>466</v>
+        <v>440</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>467</v>
+        <v>441</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>468</v>
+        <v>442</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>469</v>
+        <v>443</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="30"/>
       <c r="B9" s="23" t="s">
-        <v>470</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7362,8 +7228,8 @@
   </sheetPr>
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75390625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7373,7 +7239,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="31" t="s">
-        <v>471</v>
+        <v>444</v>
       </c>
       <c r="B1" s="31" t="n">
         <v>1</v>
@@ -7419,7 +7285,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B3" s="32" t="n">
         <v>1</v>
@@ -7442,7 +7308,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="32" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B4" s="32" t="n">
         <v>3</v>
@@ -7465,7 +7331,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="32" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B5" s="32" t="n">
         <v>3</v>
@@ -7488,7 +7354,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="32" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B6" s="32" t="n">
         <v>1</v>
@@ -7511,7 +7377,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="32" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B7" s="32" t="n">
         <v>4</v>
@@ -7534,7 +7400,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="32" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B8" s="32" t="n">
         <v>4</v>
@@ -7557,7 +7423,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="32" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="B9" s="32" t="n">
         <v>3</v>
@@ -7580,7 +7446,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="32" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B10" s="32" t="n">
         <v>2</v>
@@ -7603,7 +7469,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="32" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="B11" s="32" t="n">
         <v>3</v>
@@ -7626,7 +7492,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="32" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="B12" s="32" t="n">
         <v>2</v>
@@ -7649,7 +7515,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="B13" s="32" t="n">
         <v>6</v>
@@ -7672,7 +7538,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="32" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="B14" s="32" t="n">
         <v>4</v>
@@ -7695,7 +7561,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="32" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="B15" s="32" t="n">
         <v>4</v>
@@ -7718,7 +7584,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="32" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="B16" s="32" t="n">
         <v>3</v>
@@ -7741,7 +7607,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="32" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B17" s="32" t="n">
         <v>3</v>
@@ -7764,7 +7630,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="32" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="B18" s="32" t="n">
         <v>2</v>
@@ -7787,7 +7653,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="32" t="s">
-        <v>317</v>
+        <v>300</v>
       </c>
       <c r="B19" s="32" t="n">
         <v>3</v>
@@ -7810,7 +7676,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="32" t="s">
-        <v>326</v>
+        <v>309</v>
       </c>
       <c r="B20" s="32" t="n">
         <v>2</v>
@@ -7833,7 +7699,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="32" t="s">
-        <v>335</v>
+        <v>317</v>
       </c>
       <c r="B21" s="32" t="n">
         <v>3</v>
@@ -7856,7 +7722,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="32" t="s">
-        <v>344</v>
+        <v>325</v>
       </c>
       <c r="B22" s="32" t="n">
         <v>1</v>
@@ -7879,7 +7745,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="32" t="s">
-        <v>353</v>
+        <v>333</v>
       </c>
       <c r="B23" s="32" t="n">
         <v>4</v>
@@ -7902,7 +7768,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="32" t="s">
-        <v>360</v>
+        <v>339</v>
       </c>
       <c r="B24" s="32" t="n">
         <v>6</v>
@@ -7925,7 +7791,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="32" t="s">
-        <v>369</v>
+        <v>347</v>
       </c>
       <c r="B25" s="32" t="n">
         <v>4</v>
@@ -7948,7 +7814,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="32" t="s">
-        <v>379</v>
+        <v>356</v>
       </c>
       <c r="B26" s="32" t="n">
         <v>3</v>
@@ -7971,7 +7837,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="32" t="s">
-        <v>389</v>
+        <v>365</v>
       </c>
       <c r="B27" s="32" t="n">
         <v>1</v>
@@ -7994,7 +7860,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="32" t="s">
-        <v>398</v>
+        <v>373</v>
       </c>
       <c r="B28" s="32" t="n">
         <v>2</v>
@@ -8053,37 +7919,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="33" t="s">
-        <v>472</v>
+        <v>445</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>473</v>
+        <v>446</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>474</v>
+        <v>447</v>
       </c>
       <c r="D1" s="33" t="s">
-        <v>475</v>
+        <v>448</v>
       </c>
       <c r="E1" s="33" t="s">
-        <v>476</v>
+        <v>449</v>
       </c>
       <c r="F1" s="33" t="s">
-        <v>477</v>
+        <v>450</v>
       </c>
       <c r="G1" s="33" t="s">
-        <v>478</v>
+        <v>451</v>
       </c>
       <c r="H1" s="33" t="s">
-        <v>479</v>
+        <v>452</v>
       </c>
       <c r="I1" s="33" t="s">
-        <v>480</v>
+        <v>453</v>
       </c>
       <c r="J1" s="33" t="s">
-        <v>481</v>
+        <v>454</v>
       </c>
       <c r="K1" s="33" t="s">
-        <v>482</v>
+        <v>455</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8092,19 +7958,19 @@
       </c>
       <c r="B2" s="34"/>
       <c r="C2" s="34" t="s">
-        <v>483</v>
+        <v>456</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>484</v>
+        <v>457</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>485</v>
+        <v>458</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>486</v>
+        <v>459</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>487</v>
+        <v>460</v>
       </c>
       <c r="H2" s="34"/>
       <c r="I2" s="34"/>
@@ -8117,19 +7983,19 @@
       </c>
       <c r="B3" s="34"/>
       <c r="C3" s="34" t="s">
-        <v>488</v>
+        <v>461</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>489</v>
+        <v>462</v>
       </c>
       <c r="E3" s="34" t="s">
-        <v>490</v>
+        <v>463</v>
       </c>
       <c r="F3" s="34" t="s">
-        <v>491</v>
+        <v>464</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>487</v>
+        <v>460</v>
       </c>
       <c r="H3" s="34"/>
       <c r="I3" s="34"/>
@@ -8142,19 +8008,19 @@
       </c>
       <c r="B4" s="34"/>
       <c r="C4" s="34" t="s">
-        <v>492</v>
+        <v>465</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>493</v>
+        <v>466</v>
       </c>
       <c r="E4" s="34" t="s">
-        <v>490</v>
+        <v>463</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>494</v>
+        <v>467</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>487</v>
+        <v>460</v>
       </c>
       <c r="H4" s="34" t="s">
         <v>108</v>
@@ -8169,19 +8035,19 @@
       </c>
       <c r="B5" s="34"/>
       <c r="C5" s="34" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>496</v>
+        <v>469</v>
       </c>
       <c r="E5" s="34" t="s">
-        <v>490</v>
+        <v>463</v>
       </c>
       <c r="F5" s="34" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G5" s="34" t="s">
-        <v>487</v>
+        <v>460</v>
       </c>
       <c r="H5" s="34" t="s">
         <v>138</v>
@@ -8196,19 +8062,19 @@
       </c>
       <c r="B6" s="34"/>
       <c r="C6" s="34" t="s">
-        <v>498</v>
+        <v>471</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>499</v>
+        <v>472</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>490</v>
+        <v>463</v>
       </c>
       <c r="F6" s="34" t="s">
-        <v>500</v>
+        <v>473</v>
       </c>
       <c r="G6" s="34" t="s">
-        <v>487</v>
+        <v>460</v>
       </c>
       <c r="H6" s="34" t="s">
         <v>128</v>
@@ -8223,19 +8089,19 @@
       </c>
       <c r="B7" s="34"/>
       <c r="C7" s="34" t="s">
-        <v>501</v>
+        <v>474</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>502</v>
+        <v>475</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>490</v>
+        <v>463</v>
       </c>
       <c r="F7" s="34" t="s">
-        <v>503</v>
+        <v>476</v>
       </c>
       <c r="G7" s="34" t="s">
-        <v>487</v>
+        <v>460</v>
       </c>
       <c r="H7" s="34"/>
       <c r="I7" s="34"/>
@@ -8248,19 +8114,19 @@
       </c>
       <c r="B8" s="34"/>
       <c r="C8" s="34" t="s">
-        <v>504</v>
+        <v>477</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>505</v>
+        <v>478</v>
       </c>
       <c r="E8" s="34" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="F8" s="34" t="s">
-        <v>507</v>
+        <v>480</v>
       </c>
       <c r="G8" s="34" t="s">
-        <v>487</v>
+        <v>460</v>
       </c>
       <c r="H8" s="34" t="s">
         <v>68</v>
@@ -8275,19 +8141,19 @@
       </c>
       <c r="B9" s="34"/>
       <c r="C9" s="34" t="s">
-        <v>508</v>
+        <v>481</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>509</v>
+        <v>482</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="F9" s="34" t="s">
-        <v>507</v>
+        <v>480</v>
       </c>
       <c r="G9" s="34" t="s">
-        <v>487</v>
+        <v>460</v>
       </c>
       <c r="H9" s="34" t="s">
         <v>39</v>
@@ -8302,19 +8168,19 @@
       </c>
       <c r="B10" s="34"/>
       <c r="C10" s="34" t="s">
-        <v>510</v>
+        <v>483</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>511</v>
+        <v>484</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="F10" s="34" t="s">
-        <v>507</v>
+        <v>480</v>
       </c>
       <c r="G10" s="34" t="s">
-        <v>487</v>
+        <v>460</v>
       </c>
       <c r="H10" s="34" t="s">
         <v>21</v>
@@ -8329,19 +8195,19 @@
       </c>
       <c r="B11" s="34"/>
       <c r="C11" s="34" t="s">
-        <v>512</v>
+        <v>485</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>513</v>
+        <v>486</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="F11" s="34" t="s">
-        <v>507</v>
+        <v>480</v>
       </c>
       <c r="G11" s="34" t="s">
-        <v>514</v>
+        <v>487</v>
       </c>
       <c r="H11" s="34" t="s">
         <v>3</v>
@@ -8356,19 +8222,19 @@
       </c>
       <c r="B12" s="34"/>
       <c r="C12" s="34" t="s">
-        <v>515</v>
+        <v>488</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>516</v>
+        <v>489</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="F12" s="34" t="s">
-        <v>500</v>
+        <v>473</v>
       </c>
       <c r="G12" s="34" t="s">
-        <v>514</v>
+        <v>487</v>
       </c>
       <c r="H12" s="34" t="s">
         <v>13</v>
@@ -8383,19 +8249,19 @@
       </c>
       <c r="B13" s="34"/>
       <c r="C13" s="34" t="s">
-        <v>517</v>
+        <v>490</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>518</v>
+        <v>491</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="F13" s="34" t="s">
-        <v>500</v>
+        <v>473</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>514</v>
+        <v>487</v>
       </c>
       <c r="H13" s="34" t="s">
         <v>100</v>
@@ -8410,19 +8276,19 @@
       </c>
       <c r="B14" s="34"/>
       <c r="C14" s="34" t="s">
-        <v>519</v>
+        <v>492</v>
       </c>
       <c r="D14" s="33" t="s">
-        <v>520</v>
+        <v>493</v>
       </c>
       <c r="E14" s="34" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="F14" s="34" t="s">
-        <v>521</v>
+        <v>494</v>
       </c>
       <c r="G14" s="34" t="s">
-        <v>487</v>
+        <v>460</v>
       </c>
       <c r="H14" s="34" t="s">
         <v>76</v>
@@ -8437,19 +8303,19 @@
       </c>
       <c r="B15" s="34"/>
       <c r="C15" s="34" t="s">
-        <v>522</v>
+        <v>495</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>523</v>
+        <v>496</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="F15" s="34" t="s">
-        <v>521</v>
+        <v>494</v>
       </c>
       <c r="G15" s="34" t="s">
-        <v>514</v>
+        <v>487</v>
       </c>
       <c r="H15" s="34" t="s">
         <v>92</v>
@@ -8464,19 +8330,19 @@
       </c>
       <c r="B16" s="34"/>
       <c r="C16" s="34" t="s">
-        <v>524</v>
+        <v>497</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>525</v>
+        <v>498</v>
       </c>
       <c r="E16" s="34" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="F16" s="34" t="s">
-        <v>521</v>
+        <v>494</v>
       </c>
       <c r="G16" s="34" t="s">
-        <v>514</v>
+        <v>487</v>
       </c>
       <c r="H16" s="34" t="s">
         <v>48</v>
@@ -8491,25 +8357,25 @@
       </c>
       <c r="B17" s="34"/>
       <c r="C17" s="34" t="s">
-        <v>526</v>
+        <v>499</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>527</v>
+        <v>500</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="F17" s="34" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="G17" s="34" t="s">
-        <v>487</v>
+        <v>460</v>
       </c>
       <c r="H17" s="34"/>
       <c r="I17" s="34"/>
       <c r="J17" s="34"/>
       <c r="K17" s="33" t="s">
-        <v>529</v>
+        <v>502</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8518,19 +8384,19 @@
       </c>
       <c r="B18" s="34"/>
       <c r="C18" s="34" t="s">
-        <v>530</v>
+        <v>503</v>
       </c>
       <c r="D18" s="33" t="s">
-        <v>531</v>
+        <v>504</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="F18" s="34" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="G18" s="34" t="s">
-        <v>514</v>
+        <v>487</v>
       </c>
       <c r="H18" s="34" t="s">
         <v>84</v>
@@ -8545,25 +8411,25 @@
       </c>
       <c r="B19" s="34"/>
       <c r="C19" s="34" t="s">
-        <v>532</v>
+        <v>505</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>533</v>
+        <v>506</v>
       </c>
       <c r="E19" s="34" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="F19" s="34" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="G19" s="34" t="s">
-        <v>514</v>
+        <v>487</v>
       </c>
       <c r="H19" s="34"/>
       <c r="I19" s="34"/>
       <c r="J19" s="34"/>
       <c r="K19" s="33" t="s">
-        <v>534</v>
+        <v>507</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8572,19 +8438,19 @@
       </c>
       <c r="B20" s="34"/>
       <c r="C20" s="34" t="s">
-        <v>535</v>
+        <v>508</v>
       </c>
       <c r="D20" s="33" t="s">
-        <v>536</v>
+        <v>509</v>
       </c>
       <c r="E20" s="34" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="F20" s="34" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="G20" s="34" t="s">
-        <v>487</v>
+        <v>460</v>
       </c>
       <c r="H20" s="34" t="s">
         <v>119</v>
@@ -8599,19 +8465,19 @@
       </c>
       <c r="B21" s="34"/>
       <c r="C21" s="34" t="s">
-        <v>537</v>
+        <v>510</v>
       </c>
       <c r="D21" s="33" t="s">
-        <v>538</v>
+        <v>511</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="F21" s="34" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="G21" s="34" t="s">
-        <v>514</v>
+        <v>487</v>
       </c>
       <c r="H21" s="34" t="s">
         <v>57</v>
@@ -8626,19 +8492,19 @@
       </c>
       <c r="B22" s="34"/>
       <c r="C22" s="34" t="s">
-        <v>539</v>
+        <v>512</v>
       </c>
       <c r="D22" s="33" t="s">
-        <v>540</v>
+        <v>513</v>
       </c>
       <c r="E22" s="34" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="F22" s="34" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="G22" s="34" t="s">
-        <v>514</v>
+        <v>487</v>
       </c>
       <c r="H22" s="34" t="s">
         <v>30</v>
@@ -8646,7 +8512,7 @@
       <c r="I22" s="34"/>
       <c r="J22" s="34"/>
       <c r="K22" s="33" t="s">
-        <v>541</v>
+        <v>514</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8655,25 +8521,25 @@
       </c>
       <c r="B23" s="34"/>
       <c r="C23" s="34" t="s">
-        <v>542</v>
+        <v>515</v>
       </c>
       <c r="D23" s="33" t="s">
-        <v>543</v>
+        <v>516</v>
       </c>
       <c r="E23" s="34" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="F23" s="34" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="G23" s="34" t="s">
-        <v>514</v>
+        <v>487</v>
       </c>
       <c r="H23" s="34"/>
       <c r="I23" s="34"/>
       <c r="J23" s="34"/>
       <c r="K23" s="33" t="s">
-        <v>544</v>
+        <v>517</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8682,19 +8548,19 @@
       </c>
       <c r="B24" s="34"/>
       <c r="C24" s="34" t="s">
-        <v>545</v>
+        <v>518</v>
       </c>
       <c r="D24" s="33" t="s">
-        <v>546</v>
+        <v>519</v>
       </c>
       <c r="E24" s="34" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="F24" s="34" t="s">
-        <v>547</v>
+        <v>520</v>
       </c>
       <c r="G24" s="34" t="s">
-        <v>514</v>
+        <v>487</v>
       </c>
       <c r="H24" s="34"/>
       <c r="I24" s="34"/>
@@ -8707,19 +8573,19 @@
       </c>
       <c r="B25" s="34"/>
       <c r="C25" s="34" t="s">
-        <v>548</v>
+        <v>521</v>
       </c>
       <c r="D25" s="33" t="s">
-        <v>549</v>
+        <v>522</v>
       </c>
       <c r="E25" s="34" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="F25" s="34" t="s">
-        <v>547</v>
+        <v>520</v>
       </c>
       <c r="G25" s="34" t="s">
-        <v>487</v>
+        <v>460</v>
       </c>
       <c r="H25" s="34"/>
       <c r="I25" s="34"/>
@@ -8732,19 +8598,19 @@
       </c>
       <c r="B26" s="34"/>
       <c r="C26" s="34" t="s">
-        <v>550</v>
+        <v>523</v>
       </c>
       <c r="D26" s="33" t="s">
-        <v>551</v>
+        <v>524</v>
       </c>
       <c r="E26" s="34" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="F26" s="34" t="s">
-        <v>503</v>
+        <v>476</v>
       </c>
       <c r="G26" s="34" t="s">
-        <v>487</v>
+        <v>460</v>
       </c>
       <c r="H26" s="34"/>
       <c r="I26" s="34"/>
@@ -8757,19 +8623,19 @@
       </c>
       <c r="B27" s="34"/>
       <c r="C27" s="34" t="s">
-        <v>552</v>
+        <v>525</v>
       </c>
       <c r="D27" s="33" t="s">
-        <v>553</v>
+        <v>526</v>
       </c>
       <c r="E27" s="34" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="F27" s="34" t="s">
-        <v>503</v>
+        <v>476</v>
       </c>
       <c r="G27" s="34" t="s">
-        <v>487</v>
+        <v>460</v>
       </c>
       <c r="H27" s="34"/>
       <c r="I27" s="34"/>
@@ -8782,19 +8648,19 @@
       </c>
       <c r="B28" s="34"/>
       <c r="C28" s="34" t="s">
-        <v>554</v>
+        <v>527</v>
       </c>
       <c r="D28" s="33" t="s">
-        <v>555</v>
+        <v>528</v>
       </c>
       <c r="E28" s="34" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="F28" s="34" t="s">
-        <v>556</v>
+        <v>529</v>
       </c>
       <c r="G28" s="34" t="s">
-        <v>514</v>
+        <v>487</v>
       </c>
       <c r="H28" s="34"/>
       <c r="I28" s="34"/>
@@ -8807,19 +8673,19 @@
       </c>
       <c r="B29" s="34"/>
       <c r="C29" s="34" t="s">
-        <v>557</v>
+        <v>530</v>
       </c>
       <c r="D29" s="33" t="s">
-        <v>558</v>
+        <v>531</v>
       </c>
       <c r="E29" s="34" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="F29" s="34" t="s">
-        <v>556</v>
+        <v>529</v>
       </c>
       <c r="G29" s="34" t="s">
-        <v>487</v>
+        <v>460</v>
       </c>
       <c r="H29" s="34"/>
       <c r="I29" s="34"/>
@@ -8832,19 +8698,19 @@
       </c>
       <c r="B30" s="34"/>
       <c r="C30" s="34" t="s">
-        <v>559</v>
+        <v>532</v>
       </c>
       <c r="D30" s="33" t="s">
-        <v>560</v>
+        <v>533</v>
       </c>
       <c r="E30" s="34" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="F30" s="34" t="s">
-        <v>556</v>
+        <v>529</v>
       </c>
       <c r="G30" s="34" t="s">
-        <v>514</v>
+        <v>487</v>
       </c>
       <c r="H30" s="34"/>
       <c r="I30" s="34"/>
@@ -8857,19 +8723,19 @@
       </c>
       <c r="B31" s="34"/>
       <c r="C31" s="34" t="s">
-        <v>561</v>
+        <v>534</v>
       </c>
       <c r="D31" s="33" t="s">
-        <v>562</v>
+        <v>535</v>
       </c>
       <c r="E31" s="34" t="s">
-        <v>563</v>
+        <v>536</v>
       </c>
       <c r="F31" s="34" t="s">
-        <v>564</v>
+        <v>537</v>
       </c>
       <c r="G31" s="34" t="s">
-        <v>514</v>
+        <v>487</v>
       </c>
       <c r="H31" s="34"/>
       <c r="I31" s="34"/>
@@ -8882,19 +8748,19 @@
       </c>
       <c r="B32" s="34"/>
       <c r="C32" s="34" t="s">
-        <v>565</v>
+        <v>538</v>
       </c>
       <c r="D32" s="33" t="s">
-        <v>566</v>
+        <v>539</v>
       </c>
       <c r="E32" s="34" t="s">
-        <v>563</v>
+        <v>536</v>
       </c>
       <c r="F32" s="34" t="s">
-        <v>567</v>
+        <v>540</v>
       </c>
       <c r="G32" s="34" t="s">
-        <v>487</v>
+        <v>460</v>
       </c>
       <c r="H32" s="34"/>
       <c r="I32" s="34"/>
@@ -8907,19 +8773,19 @@
       </c>
       <c r="B33" s="34"/>
       <c r="C33" s="34" t="s">
-        <v>568</v>
+        <v>541</v>
       </c>
       <c r="D33" s="33" t="s">
-        <v>569</v>
+        <v>542</v>
       </c>
       <c r="E33" s="34" t="s">
-        <v>570</v>
+        <v>543</v>
       </c>
       <c r="F33" s="34" t="s">
-        <v>571</v>
+        <v>544</v>
       </c>
       <c r="G33" s="34" t="s">
-        <v>514</v>
+        <v>487</v>
       </c>
       <c r="H33" s="34"/>
       <c r="I33" s="34"/>
@@ -9930,7 +9796,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="35" t="s">
-        <v>572</v>
+        <v>545</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="35"/>
@@ -9951,7 +9817,7 @@
     </row>
     <row r="2" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="36" t="s">
-        <v>573</v>
+        <v>546</v>
       </c>
       <c r="B2" s="37" t="s">
         <v>3</v>
@@ -10002,60 +9868,60 @@
         <v>138</v>
       </c>
       <c r="R2" s="38" t="s">
-        <v>574</v>
+        <v>547</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="37" t="s">
-        <v>575</v>
+        <v>548</v>
       </c>
       <c r="B3" s="39" t="s">
+        <v>485</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>488</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>483</v>
+      </c>
+      <c r="E3" s="39" t="s">
         <v>512</v>
       </c>
-      <c r="C3" s="39" t="s">
-        <v>515</v>
-      </c>
-      <c r="D3" s="39" t="s">
+      <c r="F3" s="39" t="s">
+        <v>481</v>
+      </c>
+      <c r="G3" s="39" t="s">
+        <v>497</v>
+      </c>
+      <c r="H3" s="39" t="s">
         <v>510</v>
       </c>
-      <c r="E3" s="39" t="s">
-        <v>539</v>
-      </c>
-      <c r="F3" s="39" t="s">
-        <v>508</v>
-      </c>
-      <c r="G3" s="39" t="s">
-        <v>524</v>
-      </c>
-      <c r="H3" s="39" t="s">
-        <v>537</v>
-      </c>
       <c r="I3" s="39" t="s">
-        <v>504</v>
+        <v>477</v>
       </c>
       <c r="J3" s="39" t="s">
-        <v>519</v>
+        <v>492</v>
       </c>
       <c r="K3" s="39" t="s">
-        <v>530</v>
+        <v>503</v>
       </c>
       <c r="L3" s="39" t="s">
-        <v>522</v>
+        <v>495</v>
       </c>
       <c r="M3" s="39" t="s">
-        <v>517</v>
+        <v>490</v>
       </c>
       <c r="N3" s="39" t="s">
-        <v>492</v>
+        <v>465</v>
       </c>
       <c r="O3" s="39" t="s">
-        <v>501</v>
+        <v>474</v>
       </c>
       <c r="P3" s="39" t="s">
-        <v>498</v>
+        <v>471</v>
       </c>
       <c r="Q3" s="39" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="R3" s="38" t="n">
         <v>1</v>
@@ -10063,55 +9929,55 @@
     </row>
     <row r="4" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="37" t="s">
-        <v>576</v>
+        <v>549</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>537</v>
+        <v>510</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>535</v>
+        <v>508</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>539</v>
+        <v>512</v>
       </c>
       <c r="E4" s="40" t="s">
-        <v>539</v>
+        <v>512</v>
       </c>
       <c r="F4" s="40" t="s">
-        <v>535</v>
+        <v>508</v>
       </c>
       <c r="G4" s="40" t="s">
-        <v>535</v>
+        <v>508</v>
       </c>
       <c r="H4" s="40" t="s">
-        <v>537</v>
+        <v>510</v>
       </c>
       <c r="I4" s="40" t="s">
-        <v>539</v>
+        <v>512</v>
       </c>
       <c r="J4" s="40" t="s">
-        <v>530</v>
+        <v>503</v>
       </c>
       <c r="K4" s="40" t="s">
-        <v>530</v>
+        <v>503</v>
       </c>
       <c r="L4" s="40" t="s">
-        <v>537</v>
+        <v>510</v>
       </c>
       <c r="M4" s="40" t="s">
-        <v>530</v>
+        <v>503</v>
       </c>
       <c r="N4" s="40" t="s">
-        <v>488</v>
+        <v>461</v>
       </c>
       <c r="O4" s="40" t="s">
-        <v>488</v>
+        <v>461</v>
       </c>
       <c r="P4" s="40" t="s">
-        <v>488</v>
+        <v>461</v>
       </c>
       <c r="Q4" s="40" t="s">
-        <v>488</v>
+        <v>461</v>
       </c>
       <c r="R4" s="38" t="n">
         <v>2</v>
@@ -10120,55 +9986,55 @@
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="37" t="s">
-        <v>577</v>
+        <v>550</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>539</v>
+        <v>512</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>537</v>
+        <v>510</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>504</v>
+        <v>477</v>
       </c>
       <c r="E5" s="40" t="s">
-        <v>537</v>
+        <v>510</v>
       </c>
       <c r="F5" s="40" t="s">
-        <v>539</v>
+        <v>512</v>
       </c>
       <c r="G5" s="40" t="s">
-        <v>535</v>
+        <v>508</v>
       </c>
       <c r="H5" s="40" t="s">
-        <v>535</v>
+        <v>508</v>
       </c>
       <c r="I5" s="40" t="s">
-        <v>535</v>
+        <v>508</v>
       </c>
       <c r="J5" s="40" t="s">
-        <v>539</v>
+        <v>512</v>
       </c>
       <c r="K5" s="40" t="s">
-        <v>530</v>
+        <v>503</v>
       </c>
       <c r="L5" s="40" t="s">
-        <v>530</v>
+        <v>503</v>
       </c>
       <c r="M5" s="40" t="s">
-        <v>530</v>
+        <v>503</v>
       </c>
       <c r="N5" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="O5" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="P5" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="Q5" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="R5" s="38" t="n">
         <v>3</v>
@@ -10176,55 +10042,55 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="37" t="s">
-        <v>579</v>
+        <v>552</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>517</v>
+        <v>490</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>515</v>
+        <v>488</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>515</v>
+        <v>488</v>
       </c>
       <c r="E6" s="40" t="s">
-        <v>517</v>
+        <v>490</v>
       </c>
       <c r="F6" s="40" t="s">
-        <v>517</v>
+        <v>490</v>
       </c>
       <c r="G6" s="40" t="s">
-        <v>515</v>
+        <v>488</v>
       </c>
       <c r="H6" s="40" t="s">
-        <v>517</v>
+        <v>490</v>
       </c>
       <c r="I6" s="40" t="s">
-        <v>515</v>
+        <v>488</v>
       </c>
       <c r="J6" s="40" t="s">
-        <v>515</v>
+        <v>488</v>
       </c>
       <c r="K6" s="40" t="s">
-        <v>515</v>
+        <v>488</v>
       </c>
       <c r="L6" s="40" t="s">
-        <v>517</v>
+        <v>490</v>
       </c>
       <c r="M6" s="40" t="s">
-        <v>517</v>
+        <v>490</v>
       </c>
       <c r="N6" s="40" t="s">
-        <v>498</v>
+        <v>471</v>
       </c>
       <c r="O6" s="40" t="s">
-        <v>498</v>
+        <v>471</v>
       </c>
       <c r="P6" s="40" t="s">
-        <v>498</v>
+        <v>471</v>
       </c>
       <c r="Q6" s="40" t="s">
-        <v>498</v>
+        <v>471</v>
       </c>
       <c r="R6" s="38" t="n">
         <v>4</v>
@@ -10232,55 +10098,55 @@
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="37" t="s">
-        <v>580</v>
+        <v>553</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>548</v>
+        <v>521</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>545</v>
+        <v>518</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>545</v>
+        <v>518</v>
       </c>
       <c r="E7" s="40" t="s">
-        <v>548</v>
+        <v>521</v>
       </c>
       <c r="F7" s="40" t="s">
-        <v>545</v>
+        <v>518</v>
       </c>
       <c r="G7" s="40" t="s">
-        <v>548</v>
+        <v>521</v>
       </c>
       <c r="H7" s="40" t="s">
-        <v>545</v>
+        <v>518</v>
       </c>
       <c r="I7" s="40" t="s">
-        <v>548</v>
+        <v>521</v>
       </c>
       <c r="J7" s="40" t="s">
-        <v>548</v>
+        <v>521</v>
       </c>
       <c r="K7" s="40" t="s">
-        <v>548</v>
+        <v>521</v>
       </c>
       <c r="L7" s="40" t="s">
-        <v>545</v>
+        <v>518</v>
       </c>
       <c r="M7" s="40" t="s">
-        <v>545</v>
+        <v>518</v>
       </c>
       <c r="N7" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="O7" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="P7" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="Q7" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="R7" s="38" t="n">
         <v>5</v>
@@ -10288,55 +10154,55 @@
     </row>
     <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="37" t="s">
-        <v>507</v>
+        <v>480</v>
       </c>
       <c r="B8" s="40" t="s">
-        <v>512</v>
+        <v>485</v>
       </c>
       <c r="C8" s="40" t="s">
-        <v>508</v>
+        <v>481</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>510</v>
+        <v>483</v>
       </c>
       <c r="E8" s="40" t="s">
-        <v>504</v>
+        <v>477</v>
       </c>
       <c r="F8" s="40" t="s">
-        <v>508</v>
+        <v>481</v>
       </c>
       <c r="G8" s="40" t="s">
-        <v>510</v>
+        <v>483</v>
       </c>
       <c r="H8" s="40" t="s">
-        <v>510</v>
+        <v>483</v>
       </c>
       <c r="I8" s="40" t="s">
-        <v>504</v>
+        <v>477</v>
       </c>
       <c r="J8" s="40" t="s">
-        <v>512</v>
+        <v>485</v>
       </c>
       <c r="K8" s="40" t="s">
-        <v>504</v>
+        <v>477</v>
       </c>
       <c r="L8" s="40" t="s">
-        <v>512</v>
+        <v>485</v>
       </c>
       <c r="M8" s="40" t="s">
-        <v>508</v>
+        <v>481</v>
       </c>
       <c r="N8" s="40" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="O8" s="40" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="P8" s="40" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="Q8" s="40" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="R8" s="38" t="n">
         <v>6</v>
@@ -10344,55 +10210,55 @@
     </row>
     <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>581</v>
+        <v>554</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>519</v>
+        <v>492</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>522</v>
+        <v>495</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>524</v>
+        <v>497</v>
       </c>
       <c r="E9" s="40" t="s">
-        <v>522</v>
+        <v>495</v>
       </c>
       <c r="F9" s="40" t="s">
-        <v>519</v>
+        <v>492</v>
       </c>
       <c r="G9" s="40" t="s">
-        <v>524</v>
+        <v>497</v>
       </c>
       <c r="H9" s="40" t="s">
-        <v>522</v>
+        <v>495</v>
       </c>
       <c r="I9" s="40" t="s">
-        <v>524</v>
+        <v>497</v>
       </c>
       <c r="J9" s="40" t="s">
-        <v>519</v>
+        <v>492</v>
       </c>
       <c r="K9" s="40" t="s">
-        <v>524</v>
+        <v>497</v>
       </c>
       <c r="L9" s="40" t="s">
-        <v>522</v>
+        <v>495</v>
       </c>
       <c r="M9" s="40" t="s">
-        <v>519</v>
+        <v>492</v>
       </c>
       <c r="N9" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="O9" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="P9" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="Q9" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="R9" s="38" t="n">
         <v>7</v>
@@ -10400,55 +10266,55 @@
     </row>
     <row r="10" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="37" t="s">
-        <v>582</v>
+        <v>555</v>
       </c>
       <c r="B10" s="40" t="s">
-        <v>552</v>
+        <v>525</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>510</v>
+        <v>483</v>
       </c>
       <c r="D10" s="40" t="s">
-        <v>508</v>
+        <v>481</v>
       </c>
       <c r="E10" s="40" t="s">
-        <v>552</v>
+        <v>525</v>
       </c>
       <c r="F10" s="40" t="s">
-        <v>550</v>
+        <v>523</v>
       </c>
       <c r="G10" s="40" t="s">
-        <v>552</v>
+        <v>525</v>
       </c>
       <c r="H10" s="40" t="s">
-        <v>552</v>
+        <v>525</v>
       </c>
       <c r="I10" s="40" t="s">
-        <v>552</v>
+        <v>525</v>
       </c>
       <c r="J10" s="40" t="s">
-        <v>552</v>
+        <v>525</v>
       </c>
       <c r="K10" s="40" t="s">
-        <v>550</v>
+        <v>523</v>
       </c>
       <c r="L10" s="40" t="s">
-        <v>550</v>
+        <v>523</v>
       </c>
       <c r="M10" s="40" t="s">
-        <v>550</v>
+        <v>523</v>
       </c>
       <c r="N10" s="40" t="s">
-        <v>552</v>
+        <v>525</v>
       </c>
       <c r="O10" s="40" t="s">
-        <v>550</v>
+        <v>523</v>
       </c>
       <c r="P10" s="40" t="s">
-        <v>550</v>
+        <v>523</v>
       </c>
       <c r="Q10" s="40" t="s">
-        <v>552</v>
+        <v>525</v>
       </c>
       <c r="R10" s="38" t="n">
         <v>8</v>
@@ -10456,55 +10322,55 @@
     </row>
     <row r="11" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="37" t="s">
-        <v>583</v>
+        <v>556</v>
       </c>
       <c r="B11" s="40" t="s">
-        <v>557</v>
+        <v>530</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>554</v>
+        <v>527</v>
       </c>
       <c r="D11" s="40" t="s">
-        <v>554</v>
+        <v>527</v>
       </c>
       <c r="E11" s="40" t="s">
-        <v>557</v>
+        <v>530</v>
       </c>
       <c r="F11" s="40" t="s">
-        <v>557</v>
+        <v>530</v>
       </c>
       <c r="G11" s="40" t="s">
-        <v>554</v>
+        <v>527</v>
       </c>
       <c r="H11" s="40" t="s">
-        <v>554</v>
+        <v>527</v>
       </c>
       <c r="I11" s="40" t="s">
-        <v>557</v>
+        <v>530</v>
       </c>
       <c r="J11" s="40" t="s">
-        <v>554</v>
+        <v>527</v>
       </c>
       <c r="K11" s="40" t="s">
-        <v>557</v>
+        <v>530</v>
       </c>
       <c r="L11" s="40" t="s">
-        <v>557</v>
+        <v>530</v>
       </c>
       <c r="M11" s="40" t="s">
-        <v>554</v>
+        <v>527</v>
       </c>
       <c r="N11" s="40" t="s">
-        <v>554</v>
+        <v>527</v>
       </c>
       <c r="O11" s="40" t="s">
-        <v>557</v>
+        <v>530</v>
       </c>
       <c r="P11" s="40" t="s">
-        <v>557</v>
+        <v>530</v>
       </c>
       <c r="Q11" s="40" t="s">
-        <v>554</v>
+        <v>527</v>
       </c>
       <c r="R11" s="38" t="n">
         <v>9</v>
@@ -10512,19 +10378,19 @@
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="37" t="s">
-        <v>584</v>
+        <v>557</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>510</v>
+        <v>483</v>
       </c>
       <c r="C12" s="40" t="s">
-        <v>508</v>
+        <v>481</v>
       </c>
       <c r="D12" s="40" t="s">
-        <v>524</v>
+        <v>497</v>
       </c>
       <c r="E12" s="40" t="s">
-        <v>522</v>
+        <v>495</v>
       </c>
       <c r="F12" s="40"/>
       <c r="G12" s="40"/>
@@ -10542,55 +10408,55 @@
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="37" t="s">
-        <v>585</v>
+        <v>558</v>
       </c>
       <c r="B13" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="C13" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="D13" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="E13" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="F13" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="G13" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="H13" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="I13" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="J13" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="K13" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="L13" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="M13" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="N13" s="40" t="s">
-        <v>492</v>
+        <v>465</v>
       </c>
       <c r="O13" s="40" t="s">
-        <v>492</v>
+        <v>465</v>
       </c>
       <c r="P13" s="40" t="s">
-        <v>492</v>
+        <v>465</v>
       </c>
       <c r="Q13" s="40" t="s">
-        <v>492</v>
+        <v>465</v>
       </c>
       <c r="R13" s="38" t="n">
         <v>10</v>
@@ -10598,55 +10464,55 @@
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="37" t="s">
-        <v>586</v>
+        <v>559</v>
       </c>
       <c r="B14" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="C14" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="D14" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="E14" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="F14" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="G14" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="H14" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="I14" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="J14" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="K14" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="L14" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="M14" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="N14" s="40" t="s">
-        <v>587</v>
+        <v>560</v>
       </c>
       <c r="O14" s="40" t="s">
-        <v>535</v>
+        <v>508</v>
       </c>
       <c r="P14" s="40" t="s">
-        <v>535</v>
+        <v>508</v>
       </c>
       <c r="Q14" s="40" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="R14" s="38" t="n">
         <v>11</v>
@@ -10654,43 +10520,43 @@
     </row>
     <row r="15" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="37" t="s">
-        <v>588</v>
+        <v>561</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="C15" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="D15" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="E15" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="F15" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="G15" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="H15" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="I15" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="J15" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="K15" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="L15" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="M15" s="40" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="N15" s="40"/>
       <c r="O15" s="40"/>

</xml_diff>